<commit_message>
table of all specific data types by purpose
</commit_message>
<xml_diff>
--- a/visualization.xlsx
+++ b/visualization.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicatong/Documents/Data-Minimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0551C71B-B1AC-AB4A-9325-86CA76F90450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4B0575D2-5B09-DE44-96A8-A48CAC0B5FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17480" xr2:uid="{7775489A-32FA-7B4E-AD1E-32CB2ACF6ECA}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17480" activeTab="1" xr2:uid="{7775489A-32FA-7B4E-AD1E-32CB2ACF6ECA}"/>
   </bookViews>
   <sheets>
     <sheet name="ios_purposes" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="80">
   <si>
     <t xml:space="preserve">Category         </t>
   </si>
@@ -161,6 +162,105 @@
   </si>
   <si>
     <t>Developer Tools</t>
+  </si>
+  <si>
+    <t>User ID</t>
+  </si>
+  <si>
+    <t>Sensitive Info</t>
+  </si>
+  <si>
+    <t>Search History</t>
+  </si>
+  <si>
+    <t>Purchase History</t>
+  </si>
+  <si>
+    <t>Product Interaction</t>
+  </si>
+  <si>
+    <t>Precise Location</t>
+  </si>
+  <si>
+    <t>Physical Address</t>
+  </si>
+  <si>
+    <t>Photos or Videos</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>Performance Data</t>
+  </si>
+  <si>
+    <t>Payment Info</t>
+  </si>
+  <si>
+    <t>Other User Content</t>
+  </si>
+  <si>
+    <t>Other User Contact Info</t>
+  </si>
+  <si>
+    <t>Other Usage Data</t>
+  </si>
+  <si>
+    <t>Other Financial Info</t>
+  </si>
+  <si>
+    <t>Other Diagnostic Data</t>
+  </si>
+  <si>
+    <t>Other Data Types</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>Gameplay Content</t>
+  </si>
+  <si>
+    <t>Fitness</t>
+  </si>
+  <si>
+    <t>Emails or Text Messages</t>
+  </si>
+  <si>
+    <t>Email Address</t>
+  </si>
+  <si>
+    <t>Device ID</t>
+  </si>
+  <si>
+    <t>Customer Support</t>
+  </si>
+  <si>
+    <t>Credit Info</t>
+  </si>
+  <si>
+    <t>Crash Data</t>
+  </si>
+  <si>
+    <t>Contacts</t>
+  </si>
+  <si>
+    <t>Coarse Location</t>
+  </si>
+  <si>
+    <t>Browsing History</t>
+  </si>
+  <si>
+    <t>Audio Data</t>
+  </si>
+  <si>
+    <t>Advertising Data</t>
+  </si>
+  <si>
+    <t>Identifers</t>
   </si>
 </sst>
 </file>
@@ -750,12 +850,17 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t>Purposes by</a:t>
+              <a:t>Purposes x</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t> Categories</a:t>
+              <a:t> top</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Categories (number of Apps)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1658,7 +1763,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>ios Collection Purposes by Categories</a:t>
+              <a:t>ios Collection Purposes by x top Categories (by rating)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -9897,8 +10002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CABD0D29-16B8-7348-A310-D8DA5203AA8C}">
   <dimension ref="A1:AB26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView zoomScale="57" workbookViewId="0">
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10919,4 +11024,881 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1415484-0793-3A44-A308-0858D3EC5F7F}">
+  <dimension ref="A1:L33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="116" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="20.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" t="s">
+        <v>77</v>
+      </c>
+      <c r="J3" t="s">
+        <v>78</v>
+      </c>
+      <c r="L3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" t="s">
+        <v>76</v>
+      </c>
+      <c r="J4" t="s">
+        <v>77</v>
+      </c>
+      <c r="L4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" t="s">
+        <v>75</v>
+      </c>
+      <c r="J5" t="s">
+        <v>76</v>
+      </c>
+      <c r="L5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" t="s">
+        <v>74</v>
+      </c>
+      <c r="J6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" t="s">
+        <v>72</v>
+      </c>
+      <c r="J8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" t="s">
+        <v>71</v>
+      </c>
+      <c r="J9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" t="s">
+        <v>70</v>
+      </c>
+      <c r="J10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" t="s">
+        <v>67</v>
+      </c>
+      <c r="J13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" t="s">
+        <v>66</v>
+      </c>
+      <c r="G14" t="s">
+        <v>66</v>
+      </c>
+      <c r="J14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" t="s">
+        <v>65</v>
+      </c>
+      <c r="J15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" t="s">
+        <v>64</v>
+      </c>
+      <c r="J16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" t="s">
+        <v>63</v>
+      </c>
+      <c r="J17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" t="s">
+        <v>62</v>
+      </c>
+      <c r="J18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" t="s">
+        <v>61</v>
+      </c>
+      <c r="J19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20" t="s">
+        <v>60</v>
+      </c>
+      <c r="J20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21" t="s">
+        <v>59</v>
+      </c>
+      <c r="F21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21" t="s">
+        <v>59</v>
+      </c>
+      <c r="J21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" t="s">
+        <v>58</v>
+      </c>
+      <c r="G22" t="s">
+        <v>58</v>
+      </c>
+      <c r="J22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" t="s">
+        <v>57</v>
+      </c>
+      <c r="G23" t="s">
+        <v>57</v>
+      </c>
+      <c r="J23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" t="s">
+        <v>56</v>
+      </c>
+      <c r="J24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" t="s">
+        <v>55</v>
+      </c>
+      <c r="G25" t="s">
+        <v>55</v>
+      </c>
+      <c r="J25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" t="s">
+        <v>54</v>
+      </c>
+      <c r="G26" t="s">
+        <v>54</v>
+      </c>
+      <c r="J26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" t="s">
+        <v>53</v>
+      </c>
+      <c r="G27" t="s">
+        <v>53</v>
+      </c>
+      <c r="J27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" t="s">
+        <v>52</v>
+      </c>
+      <c r="G28" t="s">
+        <v>52</v>
+      </c>
+      <c r="J28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" t="s">
+        <v>51</v>
+      </c>
+      <c r="F29" t="s">
+        <v>51</v>
+      </c>
+      <c r="G29" t="s">
+        <v>51</v>
+      </c>
+      <c r="J29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" t="s">
+        <v>50</v>
+      </c>
+      <c r="G30" t="s">
+        <v>50</v>
+      </c>
+      <c r="J30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" t="s">
+        <v>49</v>
+      </c>
+      <c r="F31" t="s">
+        <v>49</v>
+      </c>
+      <c r="G31" t="s">
+        <v>49</v>
+      </c>
+      <c r="J31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" t="s">
+        <v>48</v>
+      </c>
+      <c r="E32" t="s">
+        <v>48</v>
+      </c>
+      <c r="F32" t="s">
+        <v>48</v>
+      </c>
+      <c r="G32" t="s">
+        <v>48</v>
+      </c>
+      <c r="J32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33" t="s">
+        <v>47</v>
+      </c>
+      <c r="E33" t="s">
+        <v>47</v>
+      </c>
+      <c r="F33" t="s">
+        <v>47</v>
+      </c>
+      <c r="G33" t="s">
+        <v>47</v>
+      </c>
+      <c r="J33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>